<commit_message>
EBEGU-1902 - Spalten fuer Betreuungsangebote und fuer isSchulamt und isJugendamt hinzugefuegt. Tests dafuer gemacht - Mehr Info in dem entsprechenden javadoc
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Benutzer.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Benutzer.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\hefr\vorlagen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\A$\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="975" yWindow="360" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Vorname</t>
   </si>
@@ -90,6 +90,54 @@
   </si>
   <si>
     <t>{roleGueltigBis}</t>
+  </si>
+  <si>
+    <t>Kita</t>
+  </si>
+  <si>
+    <t>Tageseltern Kleinkinder</t>
+  </si>
+  <si>
+    <t>Tageseltern Schulkinder</t>
+  </si>
+  <si>
+    <t>Tagi</t>
+  </si>
+  <si>
+    <t>Tagesschulen</t>
+  </si>
+  <si>
+    <t>Ferieninsel</t>
+  </si>
+  <si>
+    <t>Jugendamt-Angebote</t>
+  </si>
+  <si>
+    <t>Schulamt-Angebote</t>
+  </si>
+  <si>
+    <t>{isKita}</t>
+  </si>
+  <si>
+    <t>{isTageselternKleinkind}</t>
+  </si>
+  <si>
+    <t>{isTageselternSchulkind}</t>
+  </si>
+  <si>
+    <t>{isTagi}</t>
+  </si>
+  <si>
+    <t>{isTagesschule}</t>
+  </si>
+  <si>
+    <t>{isFerieninsel}</t>
+  </si>
+  <si>
+    <t>{isJugendamt}</t>
+  </si>
+  <si>
+    <t>{isSchulamt}</t>
   </si>
 </sst>
 </file>
@@ -514,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,10 +578,18 @@
     <col min="6" max="6" width="16.5703125" customWidth="1"/>
     <col min="7" max="7" width="30.140625" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" customWidth="1"/>
+    <col min="11" max="11" width="23.7109375" customWidth="1"/>
+    <col min="12" max="12" width="7.42578125" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" customWidth="1"/>
+    <col min="15" max="15" width="22.42578125" customWidth="1"/>
+    <col min="16" max="16" width="20.28515625" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -544,16 +600,32 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -566,16 +638,32 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
@@ -600,11 +688,35 @@
       <c r="H5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q5" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
@@ -630,21 +742,53 @@
         <v>10</v>
       </c>
       <c r="I6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="P6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="J6" t="s">
+      <c r="R6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
@@ -653,62 +797,126 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
EBEGU-1943: IAM_Benutzerbericht - Spalte "gültig ab"
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Benutzer.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Benutzer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\A$\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Vorname</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>{isSchulamt}</t>
+  </si>
+  <si>
+    <t>{roleGueltigAb}</t>
+  </si>
+  <si>
+    <t>Rolle gültig ab</t>
   </si>
 </sst>
 </file>
@@ -562,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,21 +581,22 @@
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
     <col min="5" max="5" width="33.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="30.140625" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" customWidth="1"/>
-    <col min="11" max="11" width="23.7109375" customWidth="1"/>
-    <col min="12" max="12" width="7.42578125" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" customWidth="1"/>
-    <col min="15" max="15" width="22.42578125" customWidth="1"/>
-    <col min="16" max="16" width="20.28515625" customWidth="1"/>
-    <col min="17" max="17" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" customWidth="1"/>
+    <col min="12" max="12" width="23.7109375" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" customWidth="1"/>
+    <col min="16" max="16" width="22.42578125" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" customWidth="1"/>
+    <col min="18" max="18" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -608,8 +615,9 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -624,8 +632,9 @@
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q2" s="3"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -646,8 +655,9 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q3" s="5"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -662,8 +672,9 @@
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q4" s="3"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
@@ -680,43 +691,46 @@
         <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="H5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="I5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="J5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="K5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="L5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="M5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="N5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="O5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="P5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="Q5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="R5" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
@@ -733,46 +747,49 @@
         <v>8</v>
       </c>
       <c r="F6" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="H6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="I6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="J6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="K6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="L6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="M6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="N6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="O6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="P6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="P6" s="10" t="s">
+      <c r="Q6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="Q6" s="10" t="s">
+      <c r="R6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -787,8 +804,9 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q7" s="3"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
@@ -805,8 +823,9 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q8" s="5"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -821,8 +840,9 @@
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q9" s="3"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -837,8 +857,9 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q10" s="3"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -853,8 +874,9 @@
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q11" s="3"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -869,8 +891,9 @@
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q12" s="3"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -885,8 +908,9 @@
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q13" s="3"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -901,8 +925,9 @@
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q14" s="3"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -917,6 +942,7 @@
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
EBEGU-2029 Namensänderung Jugendamt zu Familie & Quartier Stadt Bern
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Benutzer.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Benutzer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\EBEGU Anpassung 2018\Namensänderung\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -110,9 +110,6 @@
     <t>Ferieninsel</t>
   </si>
   <si>
-    <t>Jugendamt-Angebote</t>
-  </si>
-  <si>
     <t>Schulamt-Angebote</t>
   </si>
   <si>
@@ -144,6 +141,9 @@
   </si>
   <si>
     <t>Rolle gültig ab</t>
+  </si>
+  <si>
+    <t>Familie &amp; Quartier Angebote</t>
   </si>
 </sst>
 </file>
@@ -570,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,7 +591,7 @@
     <col min="13" max="13" width="7.42578125" customWidth="1"/>
     <col min="14" max="14" width="13.28515625" customWidth="1"/>
     <col min="15" max="15" width="14.140625" customWidth="1"/>
-    <col min="16" max="16" width="22.42578125" customWidth="1"/>
+    <col min="16" max="16" width="27.28515625" customWidth="1"/>
     <col min="17" max="17" width="20.28515625" customWidth="1"/>
     <col min="18" max="18" width="12.28515625" customWidth="1"/>
   </cols>
@@ -691,7 +691,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>20</v>
@@ -721,10 +721,10 @@
         <v>27</v>
       </c>
       <c r="P5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q5" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="R5" s="7" t="s">
         <v>13</v>
@@ -747,7 +747,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>21</v>
@@ -759,28 +759,28 @@
         <v>10</v>
       </c>
       <c r="J6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="L6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="M6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="N6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="O6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="P6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="P6" s="10" t="s">
+      <c r="Q6" s="10" t="s">
         <v>36</v>
-      </c>
-      <c r="Q6" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="R6" s="10" t="s">
         <v>11</v>

</xml_diff>